<commit_message>
Find station id by name
</commit_message>
<xml_diff>
--- a/assets/OutputData.xlsx
+++ b/assets/OutputData.xlsx
@@ -435,7 +435,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2">
+      <c r="A2" t="str">
         <v>79049004</v>
       </c>
       <c r="B2" s="1">
@@ -449,7 +449,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3">
+      <c r="A3" t="str">
         <v>79049004</v>
       </c>
       <c r="B3" s="1">
@@ -463,7 +463,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" t="str">
         <v>79049004</v>
       </c>
       <c r="B4" s="1">
@@ -477,7 +477,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" t="str">
         <v>79049004</v>
       </c>
       <c r="B5" s="1">
@@ -491,7 +491,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" t="str">
         <v>79049004</v>
       </c>
       <c r="B6" s="1">
@@ -505,7 +505,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" t="str">
         <v>79049004</v>
       </c>
       <c r="B7" s="1">
@@ -519,7 +519,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" t="str">
         <v>79049004</v>
       </c>
       <c r="B8" s="1">
@@ -533,7 +533,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" t="str">
         <v>79049004</v>
       </c>
       <c r="B9" s="1">
@@ -547,7 +547,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" t="str">
         <v>79049004</v>
       </c>
       <c r="B10" s="1">
@@ -561,7 +561,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" t="str">
         <v>79049004</v>
       </c>
       <c r="B11" s="1">
@@ -575,7 +575,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" t="str">
         <v>79049004</v>
       </c>
       <c r="B12" s="1">
@@ -589,7 +589,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" t="str">
         <v>79049004</v>
       </c>
       <c r="B13" s="1">
@@ -603,7 +603,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" t="str">
         <v>79049004</v>
       </c>
       <c r="B14" s="1">
@@ -617,7 +617,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" t="str">
         <v>79049004</v>
       </c>
       <c r="B15" s="1">
@@ -631,7 +631,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" t="str">
         <v>79049004</v>
       </c>
       <c r="B16" s="1">
@@ -645,7 +645,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17">
+      <c r="A17" t="str">
         <v>79049004</v>
       </c>
       <c r="B17" s="1">
@@ -659,7 +659,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18">
+      <c r="A18" t="str">
         <v>79049004</v>
       </c>
       <c r="B18" s="1">

</xml_diff>

<commit_message>
Add TU and other change : - .nvmrc : 16 -> 18 - Add linter ESLint and config - Add TU and coverage for SonarCloud - Review readExcel and writeExcel functions - Add processWeatherRow functions - Review Errors
</commit_message>
<xml_diff>
--- a/assets/OutputData.xlsx
+++ b/assets/OutputData.xlsx
@@ -410,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -443,27 +443,73 @@
         <v>79049004</v>
       </c>
       <c r="B2" s="1">
-        <v>44223.270833333336</v>
+        <v>45638.32013888889</v>
       </c>
       <c r="C2" s="1">
-        <v>44223.55069444444</v>
+        <v>45639.31736111111</v>
       </c>
       <c r="D2" s="2">
+        <v>-0.7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>79049004</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45639.31736111111</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45640.4375</v>
+      </c>
+      <c r="D3" s="2">
+        <v>-0.6</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.72</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>79049004</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45640.4375</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45641.34861111111</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>7.1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>4.51</v>
+      </c>
+      <c r="G4" s="2">
         <v>4.6</v>
-      </c>
-      <c r="E2" s="2">
-        <v>9.8</v>
-      </c>
-      <c r="F2" s="2">
-        <v>7.17</v>
-      </c>
-      <c r="G2" s="2">
-        <v>6.7</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
:poop:  Add TU for getWeatherDataBetween2Dates 2
</commit_message>
<xml_diff>
--- a/assets/OutputData.xlsx
+++ b/assets/OutputData.xlsx
@@ -410,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -443,73 +443,27 @@
         <v>79049004</v>
       </c>
       <c r="B2" s="1">
-        <v>45638.32013888889</v>
+        <v>45640.020833333336</v>
       </c>
       <c r="C2" s="1">
-        <v>45639.31736111111</v>
+        <v>45640.96666666667</v>
       </c>
       <c r="D2" s="2">
-        <v>-0.7</v>
+        <v>1.6</v>
       </c>
       <c r="E2" s="2">
-        <v>5.5</v>
+        <v>7.1</v>
       </c>
       <c r="F2" s="2">
-        <v>1.8</v>
+        <v>3.73</v>
       </c>
       <c r="G2" s="2">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>79049004</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45639.31736111111</v>
-      </c>
-      <c r="C3" s="1">
-        <v>45640.4375</v>
-      </c>
-      <c r="D3" s="2">
-        <v>-0.6</v>
-      </c>
-      <c r="E3" s="2">
-        <v>2.8</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.72</v>
-      </c>
-      <c r="G3" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>79049004</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45640.4375</v>
-      </c>
-      <c r="C4" s="1">
-        <v>45641.34861111111</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="E4" s="2">
-        <v>7.1</v>
-      </c>
-      <c r="F4" s="2">
-        <v>4.51</v>
-      </c>
-      <c r="G4" s="2">
-        <v>4.6</v>
+        <v>2.9</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Full rework with ChatGPT : - package.json : add axios-mock-adapter - sonar.properties : add sonar.exclusions=**/explorations/** - create and dispatch functions in differents files - Add TU by files
</commit_message>
<xml_diff>
--- a/assets/OutputData.xlsx
+++ b/assets/OutputData.xlsx
@@ -410,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -443,22 +443,22 @@
         <v>79049004</v>
       </c>
       <c r="B2" s="1">
-        <v>45638.32013888889</v>
+        <v>45669.35486111111</v>
       </c>
       <c r="C2" s="1">
-        <v>45639.31736111111</v>
+        <v>45670.31597222222</v>
       </c>
       <c r="D2" s="2">
-        <v>-0.7</v>
+        <v>-2.8</v>
       </c>
       <c r="E2" s="2">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="F2" s="2">
-        <v>1.8</v>
+        <v>0.17</v>
       </c>
       <c r="G2" s="2">
-        <v>1.3</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="3">
@@ -466,50 +466,27 @@
         <v>79049004</v>
       </c>
       <c r="B3" s="1">
-        <v>45639.31736111111</v>
+        <v>45670.31597222222</v>
       </c>
       <c r="C3" s="1">
-        <v>45640.4375</v>
+        <v>45671.336805555555</v>
       </c>
       <c r="D3" s="2">
-        <v>-0.6</v>
+        <v>-5.4</v>
       </c>
       <c r="E3" s="2">
-        <v>2.8</v>
+        <v>3.5</v>
       </c>
       <c r="F3" s="2">
-        <v>1.72</v>
+        <v>-1.48</v>
       </c>
       <c r="G3" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>79049004</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45640.4375</v>
-      </c>
-      <c r="C4" s="1">
-        <v>45641.34861111111</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="E4" s="2">
-        <v>7.1</v>
-      </c>
-      <c r="F4" s="2">
-        <v>4.51</v>
-      </c>
-      <c r="G4" s="2">
-        <v>4.6</v>
+        <v>-2</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Call script with parameters : - --excelFile - --sheetName - --firstRow 2 - --weatherStationName
</commit_message>
<xml_diff>
--- a/assets/OutputData.xlsx
+++ b/assets/OutputData.xlsx
@@ -410,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -443,22 +443,22 @@
         <v>79049004</v>
       </c>
       <c r="B2" s="1">
-        <v>45669.35486111111</v>
+        <v>45658</v>
       </c>
       <c r="C2" s="1">
-        <v>45670.31597222222</v>
+        <v>45658.25</v>
       </c>
       <c r="D2" s="2">
-        <v>-2.8</v>
+        <v>2.6</v>
       </c>
       <c r="E2" s="2">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="F2" s="2">
-        <v>0.17</v>
+        <v>3.05</v>
       </c>
       <c r="G2" s="2">
-        <v>0.3</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="3">
@@ -466,27 +466,50 @@
         <v>79049004</v>
       </c>
       <c r="B3" s="1">
-        <v>45670.31597222222</v>
+        <v>45658.25</v>
       </c>
       <c r="C3" s="1">
-        <v>45671.336805555555</v>
+        <v>45658.5</v>
       </c>
       <c r="D3" s="2">
-        <v>-5.4</v>
+        <v>2.8</v>
       </c>
       <c r="E3" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3.18</v>
+      </c>
+      <c r="G3" s="2">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>79049004</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45658.5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45658.75</v>
+      </c>
+      <c r="D4" s="2">
         <v>3.5</v>
       </c>
-      <c r="F3" s="2">
-        <v>-1.48</v>
-      </c>
-      <c r="G3" s="2">
-        <v>-2</v>
+      <c r="E4" s="2">
+        <v>4.4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3.89</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3.8</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>